<commit_message>
Interim commit on building results data Signed-off-by: Gerry Mulvenna <git@movingwifi.com>
</commit_message>
<xml_diff>
--- a/results/Mock Count spreadsheet with working out UUJ.xlsx
+++ b/results/Mock Count spreadsheet with working out UUJ.xlsx
@@ -19036,9 +19036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC26" sqref="AC26"/>
+      <selection pane="topRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>

</xml_diff>